<commit_message>
feat: add course material for w3
</commit_message>
<xml_diff>
--- a/week-2/W2-S3-FlexBox/7_Wireframing/wireframe.xlsx
+++ b/week-2/W2-S3-FlexBox/7_Wireframing/wireframe.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">logo</t>
   </si>
@@ -28,7 +28,10 @@
     <t xml:space="preserve">home</t>
   </si>
   <si>
-    <t xml:space="preserve">offering</t>
+    <t xml:space="preserve">services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact</t>
   </si>
   <si>
     <t xml:space="preserve">about</t>
@@ -76,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,25 +158,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -361,14 +373,14 @@
   <dimension ref="F1:R29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.48046875" defaultRowHeight="18.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="11.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="4.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.19"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.04"/>
@@ -383,344 +395,345 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="0"/>
-      <c r="R1" s="0"/>
+      <c r="P1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="0"/>
-      <c r="R2" s="0"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q3" s="0"/>
-      <c r="R3" s="0"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="0"/>
-      <c r="R4" s="0"/>
+      <c r="F4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="0"/>
-      <c r="R5" s="0"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="0"/>
-      <c r="R6" s="0"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="0"/>
-      <c r="R7" s="0"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="0"/>
-      <c r="R8" s="0"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q9" s="0"/>
-      <c r="R9" s="0"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="J10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="N10" s="4" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="J10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="0"/>
-      <c r="R10" s="0"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="N10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="0"/>
-      <c r="R11" s="0"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="0"/>
-      <c r="R12" s="0"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="0"/>
-      <c r="R13" s="0"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="0"/>
-      <c r="R14" s="0"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q15" s="0"/>
-      <c r="R15" s="0"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="0"/>
-      <c r="R16" s="0"/>
+      <c r="F16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="0"/>
-      <c r="R17" s="0"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="0"/>
-      <c r="R18" s="0"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="0"/>
-      <c r="R19" s="0"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="0"/>
-      <c r="R20" s="0"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q21" s="0"/>
-      <c r="R21" s="0"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
+      <c r="F22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="0"/>
-      <c r="R22" s="0"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="0"/>
-      <c r="R23" s="0"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q24" s="0"/>
-      <c r="R24" s="0"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q25" s="0"/>
+      <c r="Q25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q26" s="0"/>
+      <c r="Q26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q27" s="0"/>
+      <c r="Q27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q28" s="0"/>
+      <c r="Q28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q29" s="0"/>
+      <c r="Q29" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="J1:L1"/>
+  <mergeCells count="6">
     <mergeCell ref="F4:P8"/>
     <mergeCell ref="F10:H14"/>
     <mergeCell ref="J10:L14"/>

</xml_diff>